<commit_message>
Melhorias na API e no documento de layout
</commit_message>
<xml_diff>
--- a/docs/DesenhoLayout.xlsx
+++ b/docs/DesenhoLayout.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\PI\Group-6\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB7D950-F605-4F18-B77E-EC8EED470073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267C8CA0-D71F-4A64-9977-62584E59274F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="2" xr2:uid="{76CEAE70-0381-46A9-B65E-1E533B98B9D8}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{76CEAE70-0381-46A9-B65E-1E533B98B9D8}"/>
   </bookViews>
   <sheets>
     <sheet name="HEADER" sheetId="1" r:id="rId1"/>
-    <sheet name="LANÇAMENTOS" sheetId="2" r:id="rId2"/>
+    <sheet name="CORPO" sheetId="2" r:id="rId2"/>
     <sheet name="TRAILER" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>Campo</t>
   </si>
@@ -105,12 +105,6 @@
     <t>Quantidade registro no arquivo</t>
   </si>
   <si>
-    <t>Registro header: “1”</t>
-  </si>
-  <si>
-    <t>Registro header: “2”</t>
-  </si>
-  <si>
     <t>Nome vakinha</t>
   </si>
   <si>
@@ -184,6 +178,69 @@
   </si>
   <si>
     <t>Media de valores poder dia</t>
+  </si>
+  <si>
+    <t>72 - 72</t>
+  </si>
+  <si>
+    <t>Tamanho dos dados:</t>
+  </si>
+  <si>
+    <t>Registro corpo: “2”</t>
+  </si>
+  <si>
+    <t>1 - 1</t>
+  </si>
+  <si>
+    <t>2 - 7</t>
+  </si>
+  <si>
+    <t>8 - 52</t>
+  </si>
+  <si>
+    <t>53 - 71</t>
+  </si>
+  <si>
+    <t>2 - 31</t>
+  </si>
+  <si>
+    <t>32 - 76</t>
+  </si>
+  <si>
+    <t>77 - 176</t>
+  </si>
+  <si>
+    <t>177 - 186</t>
+  </si>
+  <si>
+    <t>187 - 194</t>
+  </si>
+  <si>
+    <t>195 - 198</t>
+  </si>
+  <si>
+    <t>199 - 206</t>
+  </si>
+  <si>
+    <t>207 - 216</t>
+  </si>
+  <si>
+    <t>217 - 224</t>
+  </si>
+  <si>
+    <t>225 - 269</t>
+  </si>
+  <si>
+    <t>270 - 279</t>
+  </si>
+  <si>
+    <t>280 - 287</t>
+  </si>
+  <si>
+    <t>2 - 6</t>
+  </si>
+  <si>
+    <t>Registro trailer: “1”</t>
   </si>
 </sst>
 </file>
@@ -242,9 +299,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -564,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E3C958-F98C-4DE4-965B-29447CF4C1EF}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,10 +678,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -628,9 +700,8 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2">
-        <f>SUM(D2:E2)</f>
-        <v>2</v>
+      <c r="D3" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E3" s="2">
         <v>6</v>
@@ -649,9 +720,8 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2">
-        <f t="shared" ref="D4:D6" si="0">SUM(D3:E3)</f>
-        <v>8</v>
+      <c r="D4" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="E4" s="2">
         <v>45</v>
@@ -670,8 +740,7 @@
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2">
-        <f t="shared" si="0"/>
+      <c r="D5" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="2">
@@ -691,9 +760,8 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2">
-        <f t="shared" si="0"/>
-        <v>72</v>
+      <c r="D6" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
@@ -702,7 +770,22 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5">
+        <f>SUM(E2:E6)</f>
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -710,10 +793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BBDCA7-CFB7-41F8-9F50-9AC11BC06332}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,14 +837,14 @@
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
-        <v>2</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -769,20 +852,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2">
-        <f>SUM(D2:E2)</f>
-        <v>3</v>
+      <c r="D3" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="E3" s="2">
         <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -790,20 +872,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2">
-        <f t="shared" ref="D4:D14" si="0">SUM(D3:E3)</f>
-        <v>33</v>
+      <c r="D4" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="E4" s="2">
         <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -811,20 +892,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2">
-        <f t="shared" si="0"/>
-        <v>78</v>
+      <c r="D5" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="E5" s="2">
         <v>100</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -832,20 +912,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2">
-        <f t="shared" si="0"/>
-        <v>178</v>
+      <c r="D6" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E6" s="2">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -853,20 +932,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2">
-        <f t="shared" si="0"/>
-        <v>188</v>
+        <v>28</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="E7" s="2">
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -874,20 +952,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2">
-        <f t="shared" si="0"/>
-        <v>196</v>
+      <c r="D8" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="E8" s="2">
         <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -895,20 +972,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="0"/>
-        <v>200</v>
+        <v>28</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,20 +992,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="2">
-        <f t="shared" si="0"/>
-        <v>208</v>
+      <c r="D10" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="E10" s="2">
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -937,20 +1012,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="0"/>
-        <v>218</v>
+        <v>28</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="E11" s="2">
         <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -958,20 +1032,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2">
-        <f t="shared" si="0"/>
-        <v>226</v>
+      <c r="D12" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="E12" s="2">
         <v>45</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -979,20 +1052,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="2">
-        <f t="shared" si="0"/>
-        <v>271</v>
+      <c r="D13" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="E13" s="2">
         <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1000,33 +1072,47 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="2">
-        <f t="shared" si="0"/>
-        <v>281</v>
+      <c r="D14" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="E14" s="2">
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>48</v>
       </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="5">
+        <f>SUM(E2:E14)</f>
+        <v>287</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:D15"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819EEE64-008D-4EAA-817B-90EFB550169A}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,14 +1152,14 @@
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
+      <c r="D2" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,9 +1172,8 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2">
-        <f>SUM(D2:E2)</f>
-        <v>2</v>
+      <c r="D3" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E3" s="2">
         <v>5</v>
@@ -1097,7 +1182,22 @@
         <v>21</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="5">
+        <f>SUM(E2:E3)</f>
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:D4"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Trocando Vakinha por Campanha no Desenho de Layout
</commit_message>
<xml_diff>
--- a/docs/DesenhoLayout.xlsx
+++ b/docs/DesenhoLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\PI\Group-6\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Luiz Dinani\Desktop\BandTec\Projetos de PI\2º ano\ONGs\Group-6\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267C8CA0-D71F-4A64-9977-62584E59274F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33582E7C-7F3C-4A00-A4C4-F6C5ED916D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{76CEAE70-0381-46A9-B65E-1E533B98B9D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{76CEAE70-0381-46A9-B65E-1E533B98B9D8}"/>
   </bookViews>
   <sheets>
     <sheet name="HEADER" sheetId="1" r:id="rId1"/>
@@ -105,18 +105,9 @@
     <t>Quantidade registro no arquivo</t>
   </si>
   <si>
-    <t>Nome vakinha</t>
-  </si>
-  <si>
-    <t>Nome da vakinha</t>
-  </si>
-  <si>
     <t>Descricao</t>
   </si>
   <si>
-    <t>Descrição da vakinha</t>
-  </si>
-  <si>
     <t>Data criação</t>
   </si>
   <si>
@@ -144,12 +135,6 @@
     <t>Ultima doação</t>
   </si>
   <si>
-    <t>Data de criação da vakinha no formato dd/MM/yyyy</t>
-  </si>
-  <si>
-    <t>Ultima doação da vakinha no formato dd/MM/yyyy</t>
-  </si>
-  <si>
     <t>Valor doação</t>
   </si>
   <si>
@@ -165,15 +150,6 @@
     <t>Previsão</t>
   </si>
   <si>
-    <t>Data prevista para terminar a vakinha</t>
-  </si>
-  <si>
-    <t>Item vakinha</t>
-  </si>
-  <si>
-    <t>Nome do item da vakinha</t>
-  </si>
-  <si>
     <t>Média</t>
   </si>
   <si>
@@ -241,6 +217,30 @@
   </si>
   <si>
     <t>Registro trailer: “1”</t>
+  </si>
+  <si>
+    <t>Nome campanha</t>
+  </si>
+  <si>
+    <t>Nome da campanha</t>
+  </si>
+  <si>
+    <t>Item campanha</t>
+  </si>
+  <si>
+    <t>Nome do item da campanha</t>
+  </si>
+  <si>
+    <t>Descrição da campanha</t>
+  </si>
+  <si>
+    <t>Data de criação da campanha no formato dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>Ultima doação da campanha no formato dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>Data prevista para terminar a campanha</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E3C958-F98C-4DE4-965B-29447CF4C1EF}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -681,7 +681,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -701,7 +701,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2">
         <v>6</v>
@@ -721,7 +721,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E4" s="2">
         <v>45</v>
@@ -741,7 +741,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2">
         <v>19</v>
@@ -761,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -796,7 +796,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,13 +838,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -852,19 +852,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E3" s="2">
         <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -872,19 +872,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2">
         <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -892,19 +892,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2">
         <v>100</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -912,19 +912,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E6" s="2">
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -932,19 +932,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E7" s="2">
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -952,19 +952,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2">
         <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -972,19 +972,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -992,19 +992,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2">
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1012,19 +1012,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E11" s="2">
         <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,19 +1032,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2">
         <v>45</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1052,19 +1052,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2">
         <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1072,24 +1072,24 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E14" s="2">
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1111,7 +1111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819EEE64-008D-4EAA-817B-90EFB550169A}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1153,13 +1153,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2">
         <v>5</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>

</xml_diff>